<commit_message>
updated shiny app and consolidated report
</commit_message>
<xml_diff>
--- a/data-raw/RMRP_2021_AI_GIS.xlsx
+++ b/data-raw/RMRP_2021_AI_GIS.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D233"/>
+  <dimension ref="A1:D235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,78 +528,73 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PE18</t>
+          <t>BO10</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Moquegua</t>
+          <t>Ingavi</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CH.AP</t>
+          <t>PE18</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Arica y Parinacota (XV)</t>
+          <t>Moquegua</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AR.CC</t>
+          <t>CH.AP</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Chaco</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>AR-H</t>
+          <t>Arica y Parinacota (XV)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CO05</t>
+          <t>AR.CC</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Antioquia</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>CO-ANT</t>
+          <t>AR-H</t>
         </is>
       </c>
     </row>
@@ -611,389 +606,394 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CO17</t>
+          <t>CO05</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Caldas</t>
+          <t>Antioquia</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CO-CAL</t>
+          <t>CO-ANT</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PY.AS</t>
+          <t>CO17</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Asunción</t>
+          <t>Caldas</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>CO-CAL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PA.PA</t>
+          <t>PY.AS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Asunción</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AW01</t>
+          <t>PA.PA</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Panama</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Guyana</t>
+          <t>Aruba</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>GY01</t>
+          <t>AW01</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Guyana</t>
+          <t>Aruba</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Guyana</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AR.SL</t>
+          <t>GY01</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>San Luis</t>
+          <t>Guyana</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CO13</t>
+          <t>AR.SL</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bolivar</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>CO-BOL</t>
+          <t>San Luis</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BR.MS</t>
+          <t>CO13</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Mato Grosso do Sul</t>
+          <t>Bolivar</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>CO-BOL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CO73</t>
+          <t>BR.MS</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Tolima</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>CO-TOL</t>
+          <t>Mato Grosso do Sul</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CL.BI</t>
+          <t>CO73</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Biobio (Viii)</t>
+          <t>Tolima</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>CO-TOL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UY.AR</t>
+          <t>CL.BI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Artigas</t>
+          <t>Biobio (Viii)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BR.RJ</t>
+          <t>UY.AR</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>Artigas</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ZZ05</t>
+          <t>BR.RJ</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BO07</t>
+          <t>ZZ05</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chile</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>AR.NQ</t>
+          <t>BO07</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>PE04</t>
+          <t>AR.NQ</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Arequipa</t>
+          <t>Neuquén</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BR.AC</t>
+          <t>PE04</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Acre</t>
+          <t>Arequipa</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>EC15</t>
+          <t>BR.AC</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Napo</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>EC-N</t>
+          <t>Acre</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>UY.RN</t>
+          <t>EC15</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Río Negro</t>
+          <t>Napo</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>EC-N</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BR.PE</t>
+          <t>UY.RN</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Pernambuco</t>
+          <t>Río Negro</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AR.CN</t>
+          <t>BR.PE</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Pernambuco</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BR.RR</t>
+          <t>AR.CN</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Roraima</t>
+          <t>Corrientes</t>
         </is>
       </c>
     </row>
@@ -1005,163 +1005,163 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>BR.SE</t>
+          <t>BR.RR</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Sergipe</t>
+          <t>Roraima</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>UY.MO</t>
+          <t>BR.SE</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Montevideo</t>
+          <t>Sergipe</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>EC19</t>
+          <t>UY.MO</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Zamora Chinchipe</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>EC-Z</t>
+          <t>Montevideo</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CO41</t>
+          <t>EC19</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Huila</t>
+          <t>Zamora Chinchipe</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>CO-HUI</t>
+          <t>EC-Z</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>AR.BA</t>
+          <t>CO41</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Buenos Aires</t>
+          <t>Huila</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>CO-HUI</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>CO47</t>
+          <t>AR.BA</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Magdalena</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>CO-MAG</t>
+          <t>Buenos Aires</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>CL.VS</t>
+          <t>CO47</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Valparaiso (V)</t>
+          <t>Magdalena</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>CO-MAG</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>PY.AG</t>
+          <t>CL.VS</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Alto Paraguay</t>
+          <t>Valparaiso (V)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>PE21</t>
+          <t>PY.AG</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Puno</t>
+          <t>Alto Paraguay</t>
         </is>
       </c>
     </row>
@@ -1173,265 +1173,260 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>PE00</t>
+          <t>PE21</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Puno</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AR.AA</t>
+          <t>PE00</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Peru</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>PY.IT</t>
+          <t>AR.AA</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Itapúa</t>
+          <t>Argentina</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>AR.LP</t>
+          <t>PY.IT</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>La Pampa</t>
+          <t>Itapúa</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>EC05</t>
+          <t>AR.LP</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Cotopaxi</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>EC-X</t>
+          <t>La Pampa</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>PY.CE</t>
+          <t>EC05</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Central</t>
+          <t>Cotopaxi</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>EC-X</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>MX.MX</t>
+          <t>PY.CE</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Central</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>EC21</t>
+          <t>MX.MX</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Sucumbios</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>EC-U</t>
+          <t>Mexico</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ZZ08</t>
+          <t>EC21</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Curacao</t>
+          <t>Sucumbios</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>EC-U</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>BO03</t>
+          <t>ZZ08</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Cochabamba</t>
+          <t>Curacao</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ZZ04</t>
+          <t>BO03</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Cochabamba</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>AR.SE</t>
+          <t>ZZ04</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Santiago del Estero</t>
+          <t>Brazil</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>BO00</t>
+          <t>AR.SE</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Santiago del Estero</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>CL.LL</t>
+          <t>BO00</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Los Lagos (X)</t>
+          <t>Bolivia</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>EC06</t>
+          <t>CL.LL</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Chimborazo</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>EC-H</t>
+          <t>Los Lagos (X)</t>
         </is>
       </c>
     </row>
@@ -1443,17 +1438,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>EC01</t>
+          <t>EC06</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Azuay</t>
+          <t>Chimborazo</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>EC-A</t>
+          <t>EC-H</t>
         </is>
       </c>
     </row>
@@ -1465,163 +1460,168 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>EC18</t>
+          <t>EC01</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Tungurahua</t>
+          <t>Azuay</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>EC-T</t>
+          <t>EC-A</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Dominican Republic</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>DO01</t>
+          <t>EC18</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Dominican Republic</t>
+          <t>Tungurahua</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>EC-T</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Dominican Republic</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>CO08</t>
+          <t>DO01</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Atlántico</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>CO-ATL</t>
+          <t>Dominican Republic</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>UY.TT</t>
+          <t>CO08</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Treinta y Tres</t>
+          <t>Atlántico</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>CO-ATL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>BR.SC</t>
+          <t>UY.TT</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Santa Catarina</t>
+          <t>Treinta y Tres</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>PY.PY</t>
+          <t>BR.SC</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Santa Catarina</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>BR.AM</t>
+          <t>PY.PY</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Amazonas</t>
+          <t>Paraguay</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>EC14</t>
+          <t>BR.AM</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Morona Santiago</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>EC-S</t>
+          <t>Amazonas</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ZZ15</t>
+          <t>EC14</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Morona Santiago</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>EC-S</t>
         </is>
       </c>
     </row>
@@ -1633,158 +1633,158 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ZZ07</t>
+          <t>ZZ15</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Peru</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>CL.TA</t>
+          <t>ZZ07</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Tarapaca (I)</t>
+          <t>Costa Rica</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>EC11</t>
+          <t>CL.TA</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Loja</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>EC-L</t>
+          <t>Tarapaca (I)</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>PE15</t>
+          <t>EC11</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Loja</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>EC-L</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>EC90</t>
+          <t>PE15</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Zona No Delimitada</t>
+          <t>Lima</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>CO68</t>
+          <t>EC90</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Santander</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>CO-SAN</t>
+          <t>Zona No Delimitada</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>UY.SA</t>
+          <t>CO68</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Salto</t>
+          <t>Santander</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>CO-SAN</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>BR.RN</t>
+          <t>UY.SA</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Rio Grande do Norte</t>
+          <t>Salto</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>AR.CB</t>
+          <t>BR.RN</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Rio Grande do Norte</t>
         </is>
       </c>
     </row>
@@ -1796,601 +1796,601 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>AR.ER</t>
+          <t>AR.CB</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Entre Ríos</t>
+          <t>Córdoba</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>BR.SP</t>
+          <t>AR.ER</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Entre Ríos</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>CO99</t>
+          <t>BR.SP</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Vichada</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>CO-VID</t>
+          <t>São Paulo</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>EC03</t>
+          <t>CO99</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Cañar</t>
+          <t>Vichada</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>EC-F</t>
+          <t>CO-VID</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>PY.PG</t>
+          <t>EC03</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Paraguarí</t>
+          <t>Cañar</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>EC-F</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>BR.RS</t>
+          <t>PY.PG</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Rio Grande do Sul</t>
+          <t>Paraguarí</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>PE08</t>
+          <t>BR.RS</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Cusco</t>
+          <t>Rio Grande do Sul</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BO00</t>
+          <t>PE08</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Cuerpo de agua</t>
+          <t>Cusco</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>AR.CH</t>
+          <t>BO11</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Chubut</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>AR-U</t>
+          <t>Cuerpo de agua</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>CL.AI</t>
+          <t>AR.CH</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Aysen Del Gen.D.C. (Xi)</t>
+          <t>Chubut</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>AR-U</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>CO81</t>
+          <t>CL.AI</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Arauca</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>CO-ARA</t>
+          <t>Aysen Del Gen.D.C. (Xi)</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>PY.NE</t>
+          <t>CO81</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Ñeembucú</t>
+          <t>Arauca</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>CO-ARA</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Curacao</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>CW01</t>
+          <t>PY.NE</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Curacao</t>
+          <t>Ñeembucú</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Curacao</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>TT01</t>
+          <t>CW01</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Curacao</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>AR.FM</t>
+          <t>TT01</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Formosa</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>BR.AL</t>
+          <t>AR.FM</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Alagoas</t>
+          <t>Formosa</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>UY.CL</t>
+          <t>BR.AL</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Cerro Largo</t>
+          <t>Alagoas</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>PE20</t>
+          <t>UY.CL</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Piura</t>
+          <t>Cerro Largo</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ZZ12</t>
+          <t>PE20</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Piura</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>AR.LR</t>
+          <t>ZZ12</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>La Rioja</t>
+          <t>Mexico</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>CO11</t>
+          <t>AR.LR</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Bogotá D.C.</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>CO-DC</t>
+          <t>La Rioja</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>PE17</t>
+          <t>CO11</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Madre De Dios</t>
+          <t>Bogotá D.C.</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>CO-DC</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>CL.CL</t>
+          <t>PE17</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Madre De Dios</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>ZZ16</t>
+          <t>CL.CL</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Chile</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>CO19</t>
+          <t>ZZ16</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Cauca</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>CO-CAU</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>CL.AT</t>
+          <t>CO19</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Atacama (Iii)</t>
+          <t>Cauca</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>CO-CAU</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>COCO</t>
+          <t>CL.AT</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Colombia</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>CO-CO</t>
+          <t>Atacama (Iii)</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>PE11</t>
+          <t>COCO</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Ica</t>
+          <t>Colombia</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>CO-CO</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>EC10</t>
+          <t>PE11</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Imbabura</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>EC-I</t>
+          <t>Ica</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>ZZ03</t>
+          <t>EC10</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Imbabura</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>EC-I</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>EC13</t>
+          <t>ZZ03</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Manabi</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>EC-M</t>
+          <t>Bolivia</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>PE01</t>
+          <t>EC13</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>Amazonas</t>
+          <t>Manabi</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>EC-M</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>UY.SJ</t>
+          <t>PE01</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Amazonas</t>
         </is>
       </c>
     </row>
@@ -2402,355 +2402,355 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>UY.LA</t>
+          <t>UY.SJ</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Lavalleja</t>
+          <t>San José</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>BO06</t>
+          <t>UY.LA</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Tarija</t>
+          <t>Lavalleja</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>PY.CY</t>
+          <t>BO06</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Canindeyú</t>
+          <t>Tarija</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>PE14</t>
+          <t>PY.CY</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Lambayeque</t>
+          <t>Canindeyú</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>PY.PH</t>
+          <t>PE14</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Presidente Hayes</t>
+          <t>Lambayeque</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>UY.FD</t>
+          <t>PY.PH</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Presidente Hayes</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>BR.DF</t>
+          <t>UY.FD</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Distrito Federal</t>
+          <t>Florida</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>AR.SA</t>
+          <t>BR.DF</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Salta</t>
+          <t>Distrito Federal</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>CO95</t>
+          <t>AR.SA</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Guaviare</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>CO-GUV</t>
+          <t>Salta</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>BO02</t>
+          <t>CO95</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>La Paz</t>
+          <t>Guaviare</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>CO-GUV</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>EC17</t>
+          <t>BO02</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Pichincha</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>EC-P</t>
+          <t>La Paz</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>BR.AP</t>
+          <t>EC17</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Amapá</t>
+          <t>Pichincha</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>EC-P</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>PY.CG</t>
+          <t>BR.AP</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Caaguazú</t>
+          <t>Amapá</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>BR.ES</t>
+          <t>PY.CG</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Espírito Santo</t>
+          <t>Caaguazú</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>EC00</t>
+          <t>BR.ES</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Ecuador</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>EC-EC</t>
+          <t>Espírito Santo</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>PY.CN</t>
+          <t>EC00</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Concepción</t>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>EC-EC</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>UY.FS</t>
+          <t>PY.CN</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>Concepción</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>BO01</t>
+          <t>UY.FS</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Chuquisaca</t>
+          <t>Flores</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>EC20</t>
+          <t>BO01</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Galapagos</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>EC-W</t>
+          <t>Chuquisaca</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>UY.DU</t>
+          <t>EC20</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Durazno</t>
+          <t>Galapagos</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>EC-W</t>
         </is>
       </c>
     </row>
@@ -2762,29 +2762,29 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>UY.TA</t>
+          <t>UY.DU</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Tacuarembó</t>
+          <t>Durazno</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>CH.ÑU</t>
+          <t>UY.TA</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Ñuble (XVI)</t>
+          <t>Tacuarembó</t>
         </is>
       </c>
     </row>
@@ -2796,487 +2796,482 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>CL.CO</t>
+          <t>CH.ÑU</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Coquimbo (Iv)</t>
+          <t>Ñuble (XVI)</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>ZZ10</t>
+          <t>CL.CO</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Coquimbo (Iv)</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>PY.GU</t>
+          <t>ZZ10</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Guairá</t>
+          <t>Ecuador</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>BR.PR</t>
+          <t>PY.GU</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Paraná</t>
+          <t>Guairá</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>AR.TF</t>
+          <t>BR.PR</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Tierra del Fuego</t>
+          <t>Paraná</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>CL.RM</t>
+          <t>AR.TF</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Metropolitana (Xiii)</t>
+          <t>Tierra del Fuego</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>CO85</t>
+          <t>CL.RM</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Casanare</t>
-        </is>
-      </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>CO-CAS</t>
+          <t>Metropolitana (Xiii)</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>BR.GO</t>
+          <t>CO85</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Goiás</t>
+          <t>Casanare</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>CO-CAS</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>UY.RV</t>
+          <t>BR.GO</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Rivera</t>
+          <t>Goiás</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>BR.PI</t>
+          <t>UY.RV</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Piauí</t>
+          <t>Rivera</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>CO27</t>
+          <t>BR.PI</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Chocó</t>
-        </is>
-      </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>CO-CHO</t>
+          <t>Piauí</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>EC24</t>
+          <t>CO27</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Santa Elena</t>
+          <t>Chocó</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>EC-SE</t>
+          <t>CO-CHO</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>AR.DF</t>
+          <t>EC24</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Ciudad de Buenos Aires</t>
+          <t>Santa Elena</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>EC-SE</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>CO88</t>
+          <t>AR.DF</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Archipielago De San Andrés</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>CO-SAP</t>
+          <t>Ciudad de Buenos Aires</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>EC08</t>
+          <t>CO88</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Esmeraldas</t>
+          <t>Archipielago De San Andrés</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>EC-E</t>
+          <t>CO-SAP</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>UY.RO</t>
+          <t>EC08</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Rocha</t>
+          <t>Esmeraldas</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>EC-E</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>CO52</t>
+          <t>UY.RO</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Nariño</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>CO-NAR</t>
+          <t>Rocha</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>PE07</t>
+          <t>CO52</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Callao</t>
+          <t>Nariño</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>CO-NAR</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>CO97</t>
+          <t>PE07</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Vaupes</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>CO-VAU</t>
+          <t>Callao</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>CL.LI</t>
+          <t>CO97</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Libertador (Vi)</t>
+          <t>Vaupes</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>CO-VAU</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>AR.CT</t>
+          <t>CL.LI</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Catamarca</t>
-        </is>
-      </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>AR-K</t>
+          <t>Libertador (Vi)</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>EC16</t>
+          <t>AR.CT</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Pastaza</t>
+          <t>Catamarca</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>EC-Y</t>
+          <t>AR-K</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>CR.CR</t>
+          <t>EC16</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Costa RIca</t>
+          <t>Pastaza</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>EC-Y</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>PE12</t>
+          <t>UY.CH</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Junin</t>
+          <t>Chuy</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>PE03</t>
+          <t>CR.CR</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Apurimac</t>
+          <t>Costa RIca</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>CO20</t>
+          <t>PE12</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>Cesar</t>
-        </is>
-      </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>CO-CES</t>
+          <t>Junin</t>
         </is>
       </c>
     </row>
@@ -3288,292 +3283,297 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>PE22</t>
+          <t>PE03</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>San Martin</t>
+          <t>Apurimac</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>PY.MI</t>
+          <t>CO20</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>Misiones</t>
+          <t>Cesar</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>CO-CES</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>AR.SJ</t>
+          <t>PE22</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>San Juan</t>
+          <t>San Martin</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>UY.PA</t>
+          <t>PY.MI</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Paysandú</t>
+          <t>Misiones</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>EC09</t>
+          <t>AR.SJ</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Guayas</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>EC-G</t>
+          <t>San Juan</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>CL.MA</t>
+          <t>UY.PA</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Magallanes (Xii)</t>
+          <t>Paysandú</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>PY.CZ</t>
+          <t>EC09</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Caazapá</t>
+          <t>Guayas</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>EC-G</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>PE16</t>
+          <t>CL.MA</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Loreto</t>
+          <t>Magallanes (Xii)</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>CO91</t>
+          <t>PY.CZ</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Amazonas</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>CO-AMA</t>
+          <t>Caazapá</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>CO86</t>
+          <t>PE16</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Putumayo</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>CO-PUT</t>
+          <t>Loreto</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>PE13</t>
+          <t>CO91</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>La Libertad</t>
+          <t>Amazonas</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>CO-AMA</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>UY.CO</t>
+          <t>CO86</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>Colonia</t>
+          <t>Putumayo</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>CO-PUT</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>EC07</t>
+          <t>PE13</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>El Oro</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>EC-O</t>
+          <t>La Libertad</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>EC23</t>
+          <t>UY.CO</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Santo Domingo De Los Tsachilas</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>EC-SD</t>
+          <t>Colonia</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>AR.MN</t>
+          <t>EC07</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Misiones</t>
+          <t>El Oro</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>EC-O</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>BR.PB</t>
+          <t>EC23</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Paraíba</t>
+          <t>Santo Domingo De Los Tsachilas</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>EC-SD</t>
         </is>
       </c>
     </row>
@@ -3585,141 +3585,136 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>AR.TM</t>
+          <t>AR.MN</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Tucumán</t>
+          <t>Misiones</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>PY.BQ</t>
+          <t>BR.PB</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Boquerón</t>
+          <t>Paraíba</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>PY.AA</t>
+          <t>AR.TM</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Alto Paraná</t>
+          <t>Tucumán</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>PE05</t>
+          <t>PY.BQ</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Ayacucho</t>
+          <t>Boquerón</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>BR.MG</t>
+          <t>PY.AA</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Minas Gerais</t>
+          <t>Alto Paraná</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>EC12</t>
+          <t>PE05</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>Los Rios</t>
-        </is>
-      </c>
-      <c r="D181" t="inlineStr">
-        <is>
-          <t>EC-R</t>
+          <t>Ayacucho</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>CO54</t>
+          <t>BR.MG</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Norte De Santander</t>
-        </is>
-      </c>
-      <c r="D182" t="inlineStr">
-        <is>
-          <t>CO-NSA</t>
+          <t>Minas Gerais</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>ZZ13</t>
+          <t>EC12</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Los Rios</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>EC-R</t>
         </is>
       </c>
     </row>
@@ -3731,39 +3726,34 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>CO23</t>
+          <t>CO54</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Norte De Santander</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>CO-COR</t>
+          <t>CO-NSA</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>EC04</t>
+          <t>ZZ13</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Carchi</t>
-        </is>
-      </c>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>EC-C</t>
+          <t>Panama</t>
         </is>
       </c>
     </row>
@@ -3775,292 +3765,302 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>CO94</t>
+          <t>CO23</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>Guainía</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>CO-GUA</t>
+          <t>CO-COR</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>AR.JY</t>
+          <t>EC04</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Jujuy</t>
+          <t>Carchi</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>EC-C</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>ZZ09</t>
+          <t>CO94</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Dominican Republic</t>
+          <t>Guainía</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>CO-GUA</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>ZZ02</t>
+          <t>AR.JY</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Aruba</t>
+          <t>Jujuy</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>CO63</t>
+          <t>ZZ09</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Quindio</t>
-        </is>
-      </c>
-      <c r="D190" t="inlineStr">
-        <is>
-          <t>CO-QUI</t>
+          <t>Dominican Republic</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>CO44</t>
+          <t>ZZ02</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>La Guajira</t>
-        </is>
-      </c>
-      <c r="D191" t="inlineStr">
-        <is>
-          <t>CO-LAG</t>
+          <t>Aruba</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>BR.MA</t>
+          <t>CO63</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Maranhão</t>
+          <t>Quindio</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>CO-QUI</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>PE19</t>
+          <t>CO44</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Pasco</t>
+          <t>La Guajira</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>CO-LAG</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>CL.AR</t>
+          <t>BR.MA</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>Araucania (Ix)</t>
+          <t>Maranhão</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>EC02</t>
+          <t>PE19</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Bolivar</t>
-        </is>
-      </c>
-      <c r="D195" t="inlineStr">
-        <is>
-          <t>EC-B</t>
+          <t>Pasco</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>BR.CE</t>
+          <t>CL.AR</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Ceará</t>
+          <t>Araucania (Ix)</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>CO15</t>
+          <t>EC02</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>Boyaca</t>
+          <t>Bolivar</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>CO-BOY</t>
+          <t>EC-B</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>AR.SC</t>
+          <t>BR.CE</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Ceará</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>PY.CR</t>
+          <t>CO15</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Cordillera</t>
+          <t>Boyaca</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>CO-BOY</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>PE06</t>
+          <t>AR.SC</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Cajamarca</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>BO05</t>
+          <t>PY.CR</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Potosí</t>
+          <t>Cordillera</t>
         </is>
       </c>
     </row>
@@ -4072,51 +4072,46 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>PE09</t>
+          <t>PE06</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Huancavelica</t>
+          <t>Cajamarca</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>BR.BA</t>
+          <t>BO05</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Bahia</t>
+          <t>Potosí</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>CO70</t>
+          <t>PE09</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Sucre</t>
-        </is>
-      </c>
-      <c r="D204" t="inlineStr">
-        <is>
-          <t>CO-SUC</t>
+          <t>Huancavelica</t>
         </is>
       </c>
     </row>
@@ -4128,97 +4123,102 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>BR.BR</t>
+          <t>BR.BA</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Bahia</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>UY.CA</t>
+          <t>CO70</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Canelones</t>
+          <t>Sucre</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>CO-SUC</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>ZZ14</t>
+          <t>BR.BR</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Brazil</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>PY.AM</t>
+          <t>UY.CA</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Amambay</t>
+          <t>Canelones</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>BO04</t>
+          <t>ZZ14</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>Oruro</t>
+          <t>Paraguay</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>PE24</t>
+          <t>PY.AM</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Tumbes</t>
+          <t>Amambay</t>
         </is>
       </c>
     </row>
@@ -4230,46 +4230,46 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>BO09</t>
+          <t>BO04</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Pando</t>
+          <t>Oruro</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>ZZ00</t>
+          <t>PE24</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Tumbes</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>BR.PA</t>
+          <t>BO09</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>Pará</t>
+          <t>Pando</t>
         </is>
       </c>
     </row>
@@ -4281,353 +4281,387 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>ZZ06</t>
+          <t>ZZ00</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Regional</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>CO50</t>
+          <t>BR.PA</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Meta</t>
-        </is>
-      </c>
-      <c r="D215" t="inlineStr">
-        <is>
-          <t>CO-MET</t>
+          <t>Pará</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>BO08</t>
+          <t>ZZ06</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>El Beni</t>
+          <t>Colombia</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>UY.SO</t>
+          <t>CO50</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Soriano</t>
+          <t>Meta</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>CO-MET</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>CL.OI</t>
+          <t>BO08</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Ocean Islands</t>
+          <t>El Beni</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>PE10</t>
+          <t>UY.SO</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Huanuco</t>
+          <t>Soriano</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>AR.RN</t>
+          <t>CL.OI</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>Río Negro</t>
+          <t>Ocean Islands</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>CL.ML</t>
+          <t>PE10</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Maule (Vii)</t>
+          <t>Huanuco</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>BR.TO</t>
+          <t>AR.RN</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>Tocantins</t>
+          <t>Río Negro</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>ZZ01</t>
+          <t>CL.ML</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Maule (Vii)</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Paraguay</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>PY.SP</t>
+          <t>BR.TO</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>San Pedro</t>
+          <t>Tocantins</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Regional</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>CO25</t>
+          <t>ZZ01</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Cundinamarca</t>
-        </is>
-      </c>
-      <c r="D225" t="inlineStr">
-        <is>
-          <t>CO-CUN</t>
+          <t>Argentina</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Paraguay</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>AR.SF</t>
+          <t>PY.SP</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Santa Fe</t>
+          <t>San Pedro</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Uruguay</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>UY.MA</t>
+          <t>CO25</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>Maldonado</t>
+          <t>Cundinamarca</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>CO-CUN</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>CO18</t>
+          <t>AR.SF</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Caquetá</t>
-        </is>
-      </c>
-      <c r="D228" t="inlineStr">
-        <is>
-          <t>CO-CAQ</t>
+          <t>Santa Fe</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Uruguay</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>AR.MZ</t>
+          <t>UY.MA</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Mendoza</t>
+          <t>Maldonado</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>CL.AN</t>
+          <t>CO18</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Antofagasta (Ii)</t>
+          <t>Caquetá</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>CO-CAQ</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>BR.MT</t>
+          <t>AR.MZ</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Mato Grosso</t>
+          <t>Mendoza</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>CO66</t>
+          <t>CL.AN</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Risaralda</t>
-        </is>
-      </c>
-      <c r="D232" t="inlineStr">
-        <is>
-          <t>CO-RIS</t>
+          <t>Antofagasta (Ii)</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
+          <t>Brazil</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>BR.MT</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Mato Grosso</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>CO66</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>Risaralda</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>CO-RIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
           <t>Uruguay</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr">
+      <c r="B235" t="inlineStr">
         <is>
           <t>UY.UY</t>
         </is>
       </c>
-      <c r="C233" t="inlineStr">
+      <c r="C235" t="inlineStr">
         <is>
           <t>Uruguay</t>
         </is>

</xml_diff>